<commit_message>
Schemas 5,6,7,9,10,11,12,13 y 1 días válidos
</commit_message>
<xml_diff>
--- a/empresas_con_descripcion_corto.xlsx
+++ b/empresas_con_descripcion_corto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
   <si>
     <t xml:space="preserve">MANUNTENCIONES HIDROELEVACION S.L.</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">https://img.pixers.pics/pho_wat(s3:700/FO/14/31/98/62/700_FO14319862_15159f131b8bdf481b88b93c6cd7bd9f.jpg,700,466,cms:2018/10/5bd1b6b8d04b8_220x50-watermark.png,over,480,416,jpg)/vinilos-culo-mujer-evaluandola-rosa-g-string-bikini.jpg.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;li&gt;&lt;div class="collapse" id="horario5"&gt;&lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Sa 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;/div&gt;&lt;/li&gt;</t>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario5"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">MANUNTENCIONES HIDROELEVACION S.L. ofrece servicios especializados en alquiler de maquinaria y equipos profesionales en A Coruña, nan. Somos referentes en el sector de CARRETILLAS ELEVADORAS: REPARACION, proporcionando soluciones de renta de maquinaria industrial para trabajos de construcción, mantenimiento y proyectos técnicos. Contamos con maquinaria profesional para actividades como [], adaptada a las necesidades de empresas y autónomos. Nuestro catálogo incluye marcas de calidad como [], garantizando rendimiento y fiabilidad. Si buscas servicios de alquiler en A Coruña con asesoramiento experto y disponibilidad inmediata, somos tu mejor opción en la provincia de nan.</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">//estaticos.paginasamarillas.es/paginasamarillas/9_11_2/ficha/images/empty.png</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;li&gt;&lt;div class="collapse" id="horario6"&gt;&lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;/div&gt;&lt;/li&gt;</t>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario6"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">SANDE Y DIAZ ofrece servicios especializados en alquiler de maquinaria y equipos profesionales en A Coruña, nan. Somos referentes en el sector de COMPRESORES: FABRICACION, proporcionando soluciones de renta de maquinaria industrial para trabajos de construcción, mantenimiento y proyectos técnicos. Contamos con maquinaria profesional para actividades como [], adaptada a las necesidades de empresas y autónomos. Nuestro catálogo incluye marcas de calidad como [], garantizando rendimiento y fiabilidad. Si buscas servicios de alquiler en A Coruña con asesoramiento experto y disponibilidad inmediata, somos tu mejor opción en la provincia de nan.</t>
@@ -121,10 +121,46 @@
     <t xml:space="preserve">&lt;iframe src='https://www.google.com/maps?q=42.7642018,-8.2675955&amp;z=15&amp;output=embed' width='600' height='450' style='border:0;' allowfullscreen loading='lazy' referrerpolicy='no-referrer-when-downgrade'&gt;&lt;/iframe&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;li&gt;&lt;div class="collapse" id="horario7"&gt;&lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;/div&gt;&lt;/li&gt;</t>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario7"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Domingo&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Su 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Gruas Y Talleres Fuerte ofrece servicios especializados en alquiler de maquinaria y equipos profesionales en Vila de Cruces, Pontevedra. Somos referentes en el sector de GRUAS PARA CONSTRUCCION E INDUSTRIA: VENTA Y ALQUILER, proporcionando soluciones de renta de maquinaria industrial para trabajos de construcción, mantenimiento y proyectos técnicos. Contamos con maquinaria profesional para actividades como [], adaptada a las necesidades de empresas y autónomos. Nuestro catálogo incluye marcas de calidad como [], garantizando rendimiento y fiabilidad. Si buscas servicios de alquiler en Vila de Cruces con asesoramiento experto y disponibilidad inmediata, somos tu mejor opción en la provincia de Pontevedra.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario9"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;s&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grande y Díaz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario10"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gruas taller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario11"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hidro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario12"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Sa 16:45-22:45"&gt;16:45-22:45&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diazsand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario13"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Sa 16:45-22:45"&gt;16:45-22:45&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Domingo&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt; &lt;/div&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;li&gt; &lt;div class="collapse" id="horario14"&gt; &lt;p&gt;&lt;b&gt;Lunes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Mo 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Mo 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Martes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Tu 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Tu 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Miércoles&lt;/b&gt;&lt;time itemprop="openingHours" datetime="We 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="We 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Jueves&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Th 09:00-13:00"&gt;09:00-13:00&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Th 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Viernes&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Fr 09:00-13:00"&gt;09:00-13:00&lt;/time&gt; y &lt;time itemprop="openingHours" datetime="Fr 16:00-20:00"&gt;16:00-20:00&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Sábado&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Sa 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Sa 16:45-22:45"&gt;16:45-22:45&lt;/time&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;Domingo&lt;/b&gt;&lt;time itemprop="openingHours" datetime="Su 09:00-13:00"&gt; 9:35-14:45&lt;/time&gt;y &lt;time itemprop="openingHours" datetime="Su 16:45-22:45"&gt;16:45-22:45&lt;/time&gt;&lt;/p&gt; &lt;/div&gt;&lt;/li&gt;</t>
   </si>
 </sst>
 </file>
@@ -206,7 +242,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +253,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -342,10 +382,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R3" activeCellId="0" sqref="R3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -368,7 +408,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="1" width="296.22"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,14 +445,14 @@
       <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -452,14 +492,14 @@
       <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -499,16 +539,294 @@
       <c r="M3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="S3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M1" r:id="rId1" display="https://img.pixers.pics/pho_wat(s3:700/FO/14/31/98/62/700_FO14319862_15159f131b8bdf481b88b93c6cd7bd9f.jpg,700,466,cms:2018/10/5bd1b6b8d04b8_220x50-watermark.png,over,480,416,jpg)/vinilos-culo-mujer-evaluandola-rosa-g-string-bikini.jpg.jpg"/>
+    <hyperlink ref="M4" r:id="rId2" display="https://img.pixers.pics/pho_wat(s3:700/FO/14/31/98/62/700_FO14319862_15159f131b8bdf481b88b93c6cd7bd9f.jpg,700,466,cms:2018/10/5bd1b6b8d04b8_220x50-watermark.png,over,480,416,jpg)/vinilos-culo-mujer-evaluandola-rosa-g-string-bikini.jpg.jpg"/>
+    <hyperlink ref="M7" r:id="rId3" display="https://img.pixers.pics/pho_wat(s3:700/FO/14/31/98/62/700_FO14319862_15159f131b8bdf481b88b93c6cd7bd9f.jpg,700,466,cms:2018/10/5bd1b6b8d04b8_220x50-watermark.png,over,480,416,jpg)/vinilos-culo-mujer-evaluandola-rosa-g-string-bikini.jpg.jpg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ficha de negocio en municipio creada. Hay que mirar la web
</commit_message>
<xml_diff>
--- a/empresas_con_descripcion_corto.xlsx
+++ b/empresas_con_descripcion_corto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
   <si>
     <t xml:space="preserve">MANUNTENCIONES HIDROELEVACION S.L.</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">A Coruña</t>
   </si>
   <si>
-    <t xml:space="preserve">609170713.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">CARRETILLAS ELEVADORAS: REPARACION</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t xml:space="preserve">15006.0</t>
   </si>
   <si>
-    <t xml:space="preserve">981174209.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">http://www.sandeydiaz.com?utm_campaign=paginasamarillas&amp;utm_source=paginasamarillas&amp;utm_medium=referral</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pontevedra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">986583547.0</t>
   </si>
   <si>
     <t xml:space="preserve">http://gruasfuerte.com?utm_campaign=paginasamarillas&amp;utm_source=paginasamarillas&amp;utm_medium=referral</t>
@@ -167,8 +158,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -242,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -251,11 +243,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -385,7 +381,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -424,131 +420,131 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="n">
+        <v>609170713</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="R1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>981174209</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="R2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="2" t="n">
+        <v>986583547</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
@@ -562,131 +558,131 @@
       <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="n">
+        <v>609170713</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>36</v>
+      <c r="R4" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>981174209</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="R5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="2" t="n">
+        <v>986583547</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
@@ -700,126 +696,126 @@
       <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="n">
+        <v>609170713</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>42</v>
+      <c r="R7" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>981174209</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="R8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="2" t="n">
+        <v>986583547</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>